<commit_message>
Fixed type in Cards + added rules doc
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -119,6 +119,9 @@
     <t>Artillary</t>
   </si>
   <si>
+    <t>Attacks deal cone shaped damage</t>
+  </si>
+  <si>
     <t>Basic Hire</t>
   </si>
   <si>
@@ -138,9 +141,6 @@
   </si>
   <si>
     <t>Deal 3 damage to target</t>
-  </si>
-  <si>
-    <t>Attacks deal cone shaped damage if target was a unit</t>
   </si>
   <si>
     <t>Has indirrect attacks</t>
@@ -536,7 +536,7 @@
   <dimension ref="A1:N104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,7 +983,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>18</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>27</v>
@@ -1071,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>18</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>27</v>
@@ -1115,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>18</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>27</v>
@@ -1159,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>18</v>

</xml_diff>